<commit_message>
Performed calibration and implemented automation of Data Matrices file.
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Jig_Calibration_08-05-20/08-05-20_JigCalibration_results_0deg.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Jig_Calibration_08-05-20/08-05-20_JigCalibration_results_0deg.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\AMIRo\FBG_Needle_Calibration_Data\needle_3CH_4AA\Jig_Calibration_08-05-20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C03552-EEF0-4B82-B092-6490647B9564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B383B62D-AF75-4385-BBE3-AB532EC65D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="23610" windowHeight="12930" firstSheet="7" activeTab="8" xr2:uid="{CAC25A53-9E65-49F7-973B-C9FEADB2C5CC}"/>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="23610" windowHeight="12930" firstSheet="5" activeTab="8" xr2:uid="{3EED0241-C1DA-4213-BFC6-10B5DE936DFF}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="23610" windowHeight="12930" xr2:uid="{CAC25A53-9E65-49F7-973B-C9FEADB2C5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Summary" sheetId="5" r:id="rId1"/>
@@ -144,10 +143,10 @@
     <t>CH3 | AA4</t>
   </si>
   <si>
-    <t>AA$</t>
+    <t>Active Area 4</t>
   </si>
   <si>
-    <t>Active Area 4</t>
+    <t>AA4</t>
   </si>
 </sst>
 </file>
@@ -19130,8 +19129,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D376E154-FEB7-4F67-92EA-C4111B537857}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="102" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19142,8 +19140,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D0D76D07-F4E7-4196-8E52-578F166A6949}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="102" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19154,8 +19151,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{89EFA366-3CC5-4D0D-8321-22B9B883BD20}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="102" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19166,8 +19162,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CF5A8BA8-89FD-4A76-8633-757E78538492}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="90" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19178,8 +19173,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{62DDA35D-73B2-4F75-B2FA-777EFF548614}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="90" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19190,8 +19184,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AE4E7A9A-572F-4371-9659-2B807B9650CC}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="90" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19203,7 +19196,6 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
-    <sheetView zoomScale="90" workbookViewId="1" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19214,8 +19206,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B6E327A5-2F35-42F7-A4DD-34AF8D828FA5}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0" zoomToFit="1"/>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="1" zoomToFit="1"/>
+    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19226,7 +19217,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8673171" cy="6295793"/>
+    <xdr:ext cx="8657167" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -19259,7 +19250,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665882" cy="6293971"/>
+    <xdr:ext cx="8657167" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -19292,7 +19283,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665882" cy="6293971"/>
+    <xdr:ext cx="8657167" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -19940,11 +19931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D5E9E2-F53E-442B-814A-AA14022BCEF8}">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
-    </sheetView>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="Y14" sqref="Y14:Y20"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14:AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19978,7 +19966,7 @@
       <c r="U1" s="14"/>
       <c r="V1" s="14"/>
       <c r="Y1" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z1" s="14"/>
       <c r="AA1" s="14"/>
@@ -19998,7 +19986,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -20831,7 +20819,7 @@
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
       <c r="Y12" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
@@ -21372,9 +21360,6 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-    <sheetView topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="1">
-      <selection activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>